<commit_message>
fin données exo 2023
</commit_message>
<xml_diff>
--- a/Data/exogeneous_variables.xlsx
+++ b/Data/exogeneous_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\Github\GitHub\GQ-2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277E9DDB-D3AA-4F37-822A-C094C3A623A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CCDD76-1A8F-4022-86D9-50F0BA5E1FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D46BF8A0-ACDA-45E6-BD99-A97EEDCCBAF0}"/>
   </bookViews>
@@ -81,18 +81,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,16 +101,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -459,7 +450,7 @@
   <dimension ref="A1:J589"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -473,25 +464,25 @@
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -12560,8 +12551,14 @@
       <c r="F386" s="2">
         <v>1.9710000000000001</v>
       </c>
+      <c r="G386" s="2">
+        <v>0.43280000000000002</v>
+      </c>
       <c r="H386" s="2">
         <v>0.09</v>
+      </c>
+      <c r="I386" s="2">
+        <v>-0.1969565217391305</v>
       </c>
       <c r="J386" s="2">
         <v>0.9399999999999995</v>
@@ -12586,8 +12583,14 @@
       <c r="F387" s="2">
         <v>-1.3069999999999999</v>
       </c>
+      <c r="G387" s="2">
+        <v>0.38370000000000004</v>
+      </c>
       <c r="H387" s="2">
         <v>0.20760000000000001</v>
+      </c>
+      <c r="I387" s="2">
+        <v>-0.28899999999999992</v>
       </c>
       <c r="J387" s="2">
         <v>0.89000000000000057</v>
@@ -12612,8 +12615,14 @@
       <c r="F388" s="2">
         <v>0.86599999999999999</v>
       </c>
+      <c r="G388" s="2">
+        <v>0.42570000000000002</v>
+      </c>
       <c r="H388" s="2">
         <v>0.126</v>
+      </c>
+      <c r="I388" s="2">
+        <v>-0.37454545454545463</v>
       </c>
       <c r="J388" s="2">
         <v>0.96999999999999975</v>
@@ -12638,8 +12647,14 @@
       <c r="F389" s="2">
         <v>3.944</v>
       </c>
+      <c r="G389" s="2">
+        <v>0.43480000000000002</v>
+      </c>
       <c r="H389" s="2">
         <v>0.1033</v>
+      </c>
+      <c r="I389" s="2">
+        <v>-0.17523809523809511</v>
       </c>
       <c r="J389" s="2">
         <v>0.91999999999999993</v>
@@ -12664,8 +12679,14 @@
       <c r="F390" s="2">
         <v>3.7049999999999996</v>
       </c>
+      <c r="G390" s="2">
+        <v>0.40460000000000002</v>
+      </c>
       <c r="H390" s="2">
         <v>0.21029999999999999</v>
+      </c>
+      <c r="I390" s="2">
+        <v>1.304347826086967E-2</v>
       </c>
       <c r="J390" s="2">
         <v>0.91999999999999993</v>
@@ -12690,8 +12711,14 @@
       <c r="F391" s="2">
         <v>-1.6900000000000002</v>
       </c>
+      <c r="G391" s="2">
+        <v>0.39179999999999998</v>
+      </c>
       <c r="H391" s="2">
         <v>0.11280000000000001</v>
+      </c>
+      <c r="I391" s="2">
+        <v>0.49190476190476201</v>
       </c>
       <c r="J391" s="2">
         <v>0.91000000000000014</v>
@@ -12716,8 +12743,14 @@
       <c r="F392" s="2">
         <v>-3.617</v>
       </c>
+      <c r="G392" s="2">
+        <v>0.3962</v>
+      </c>
       <c r="H392" s="2">
         <v>0.10250000000000001</v>
+      </c>
+      <c r="I392" s="2">
+        <v>0.1745454545454547</v>
       </c>
       <c r="J392" s="2">
         <v>0.91999999999999993</v>
@@ -12742,8 +12775,14 @@
       <c r="F393" s="2">
         <v>1.4</v>
       </c>
+      <c r="G393" s="2">
+        <v>0.42050000000000004</v>
+      </c>
       <c r="H393" s="2">
         <v>0.19620000000000001</v>
+      </c>
+      <c r="I393" s="2">
+        <v>0.47304347826086951</v>
       </c>
       <c r="J393" s="2">
         <v>0.86000000000000032</v>
@@ -12768,8 +12807,14 @@
       <c r="F394" s="2">
         <v>3.3940000000000006</v>
       </c>
+      <c r="G394" s="2">
+        <v>0.3347</v>
+      </c>
       <c r="H394" s="2">
         <v>0.13370000000000001</v>
+      </c>
+      <c r="I394" s="2">
+        <v>0.59800000000000009</v>
       </c>
       <c r="J394" s="2">
         <v>0.84999999999999964</v>
@@ -12794,8 +12839,14 @@
       <c r="F395" s="2">
         <v>1.802</v>
       </c>
+      <c r="G395" s="2">
+        <v>0.32119999999999999</v>
+      </c>
       <c r="H395" s="2">
         <v>0.10490000000000001</v>
+      </c>
+      <c r="I395" s="2">
+        <v>0.60086956521739143</v>
       </c>
       <c r="J395" s="2">
         <v>0.82000000000000028</v>
@@ -12820,8 +12871,14 @@
       <c r="F396" s="2">
         <v>-5.5750000000000002</v>
       </c>
+      <c r="G396" s="2">
+        <v>0.33950000000000002</v>
+      </c>
       <c r="H396" s="2">
         <v>0.19700000000000001</v>
+      </c>
+      <c r="I396" s="2">
+        <v>0.79590909090909101</v>
       </c>
       <c r="J396" s="2">
         <v>0.96</v>
@@ -12846,8 +12903,14 @@
       <c r="F397" s="2">
         <v>-2.0060000000000007</v>
       </c>
+      <c r="G397" s="2">
+        <v>0.29210000000000003</v>
+      </c>
       <c r="H397" s="2">
         <v>0.158</v>
+      </c>
+      <c r="I397" s="2">
+        <v>1.04952380952381</v>
       </c>
       <c r="J397" s="2">
         <v>1.1600000000000001</v>
@@ -12872,8 +12935,14 @@
       <c r="F398" s="2">
         <v>-4.2370000000000001</v>
       </c>
+      <c r="G398" s="2">
+        <v>0.24299999999999999</v>
+      </c>
       <c r="H398" s="2">
         <v>0.11080000000000001</v>
+      </c>
+      <c r="I398" s="2">
+        <v>0.90478260869565208</v>
       </c>
       <c r="J398" s="2">
         <v>1.21</v>
@@ -12898,8 +12967,14 @@
       <c r="F399" s="2">
         <v>-4.4760000000000009</v>
       </c>
+      <c r="G399" s="2">
+        <v>0.13250000000000001</v>
+      </c>
       <c r="H399" s="2">
         <v>0.20100000000000001</v>
+      </c>
+      <c r="I399" s="2">
+        <v>1.5361904761904761</v>
       </c>
       <c r="J399" s="2">
         <v>1.29</v>
@@ -12924,8 +12999,14 @@
       <c r="F400" s="2">
         <v>-2.1989999999999998</v>
       </c>
+      <c r="G400" s="2">
+        <v>0.18690000000000001</v>
+      </c>
       <c r="H400" s="2">
         <v>0.14760000000000001</v>
+      </c>
+      <c r="I400" s="2">
+        <v>2.14047619047619</v>
       </c>
       <c r="J400" s="2">
         <v>1.38</v>
@@ -12950,8 +13031,14 @@
       <c r="F401" s="2">
         <v>5.335</v>
       </c>
+      <c r="G401" s="2">
+        <v>0.10250000000000001</v>
+      </c>
       <c r="H401" s="2">
         <v>0.10440000000000001</v>
+      </c>
+      <c r="I401" s="2">
+        <v>2.3813636363636359</v>
       </c>
       <c r="J401" s="2">
         <v>1.42</v>
@@ -12976,8 +13063,14 @@
       <c r="F402" s="2">
         <v>1.2769999999999999</v>
       </c>
+      <c r="G402" s="2">
+        <v>9.4600000000000004E-2</v>
+      </c>
       <c r="H402" s="2">
         <v>0.2077</v>
+      </c>
+      <c r="I402" s="2">
+        <v>2.0486363636363638</v>
       </c>
       <c r="J402" s="2">
         <v>1.3599999999999994</v>
@@ -13002,8 +13095,14 @@
       <c r="F403" s="2">
         <v>-10.934999999999999</v>
       </c>
+      <c r="G403" s="2">
+        <v>0.17500000000000002</v>
+      </c>
       <c r="H403" s="2">
         <v>0.14760000000000001</v>
+      </c>
+      <c r="I403" s="2">
+        <v>2.2433333333333332</v>
       </c>
       <c r="J403" s="2">
         <v>1.3900000000000006</v>
@@ -13028,8 +13127,14 @@
       <c r="F404" s="2">
         <v>0.57400000000000007</v>
       </c>
+      <c r="G404" s="2">
+        <v>0.14400000000000002</v>
+      </c>
       <c r="H404" s="2">
         <v>0.12990000000000002</v>
+      </c>
+      <c r="I404" s="2">
+        <v>2.2782608695652171</v>
       </c>
       <c r="J404" s="2">
         <v>1.4900000000000002</v>
@@ -13054,8 +13159,14 @@
       <c r="F405" s="2">
         <v>1.466</v>
       </c>
+      <c r="G405" s="2">
+        <v>0.12819999999999998</v>
+      </c>
       <c r="H405" s="2">
         <v>0.20249999999999999</v>
+      </c>
+      <c r="I405" s="2">
+        <v>2.1638095238095238</v>
       </c>
       <c r="J405" s="2">
         <v>1.5100000000000007</v>
@@ -13080,8 +13191,14 @@
       <c r="F406" s="2">
         <v>-10.284000000000001</v>
       </c>
+      <c r="G406" s="2">
+        <v>0.153</v>
+      </c>
       <c r="H406" s="2">
         <v>0.15969999999999998</v>
+      </c>
+      <c r="I406" s="2">
+        <v>2.435909090909091</v>
       </c>
       <c r="J406" s="2">
         <v>1.6599999999999993</v>
@@ -13106,8 +13223,14 @@
       <c r="F407" s="2">
         <v>-18.475000000000001</v>
       </c>
+      <c r="G407" s="2">
+        <v>7.9199999999999993E-2</v>
+      </c>
       <c r="H407" s="2">
         <v>0.1401</v>
+      </c>
+      <c r="I407" s="2">
+        <v>3.003043478260869</v>
       </c>
       <c r="J407" s="2">
         <v>2.6000000000000005</v>
@@ -13132,8 +13255,14 @@
       <c r="F408" s="2">
         <v>-9.5739999999999998</v>
       </c>
+      <c r="G408" s="2">
+        <v>2.2800000000000001E-2</v>
+      </c>
       <c r="H408" s="2">
         <v>0.2732</v>
+      </c>
+      <c r="I408" s="2">
+        <v>3.0019999999999998</v>
       </c>
       <c r="J408" s="2">
         <v>3.0900000000000007</v>
@@ -13158,8 +13287,14 @@
       <c r="F409" s="2">
         <v>2.8040000000000003</v>
       </c>
+      <c r="G409" s="2">
+        <v>2.8999999999999998E-3</v>
+      </c>
       <c r="H409" s="2">
         <v>0.23679999999999998</v>
+      </c>
+      <c r="I409" s="2">
+        <v>2.2782608695652171</v>
       </c>
       <c r="J409" s="2">
         <v>3.38</v>
@@ -13184,8 +13319,14 @@
       <c r="F410" s="2">
         <v>-8.4599999999999991</v>
       </c>
+      <c r="G410" s="2">
+        <v>2.3E-3</v>
+      </c>
       <c r="H410" s="2">
         <v>0.13489999999999999</v>
+      </c>
+      <c r="I410" s="2">
+        <v>2.170454545454545</v>
       </c>
       <c r="J410" s="2">
         <v>3.0900000000000007</v>
@@ -13210,8 +13351,14 @@
       <c r="F411" s="2">
         <v>-12.069999999999999</v>
       </c>
+      <c r="G411" s="2">
+        <v>1.47E-2</v>
+      </c>
       <c r="H411" s="2">
         <v>0.3327</v>
+      </c>
+      <c r="I411" s="2">
+        <v>2.4455</v>
       </c>
       <c r="J411" s="2">
         <v>2.8100000000000005</v>
@@ -13236,8 +13383,14 @@
       <c r="F412" s="2">
         <v>13.706</v>
       </c>
+      <c r="G412" s="2">
+        <v>1.5899999999999997E-2</v>
+      </c>
       <c r="H412" s="2">
         <v>0.30059999999999998</v>
+      </c>
+      <c r="I412" s="2">
+        <v>2.605909090909091</v>
       </c>
       <c r="J412" s="2">
         <v>2.92</v>
@@ -13262,8 +13415,14 @@
       <c r="F413" s="2">
         <v>18.937000000000001</v>
       </c>
+      <c r="G413" s="2">
+        <v>1.2500000000000001E-2</v>
+      </c>
       <c r="H413" s="2">
         <v>0.15820000000000001</v>
+      </c>
+      <c r="I413" s="2">
+        <v>2.6431818181818181</v>
       </c>
       <c r="J413" s="2">
         <v>3.0000000000000009</v>
@@ -13288,8 +13447,14 @@
       <c r="F414" s="2">
         <v>8.5250000000000004</v>
       </c>
+      <c r="G414" s="2">
+        <v>1.6999999999999999E-3</v>
+      </c>
       <c r="H414" s="2">
         <v>0.25030000000000002</v>
+      </c>
+      <c r="I414" s="2">
+        <v>2.9685714285714289</v>
       </c>
       <c r="J414" s="2">
         <v>2.5200000000000005</v>
@@ -13314,8 +13479,14 @@
       <c r="F415" s="2">
         <v>-0.74900000000000033</v>
       </c>
+      <c r="G415" s="2">
+        <v>7.4999999999999997E-3</v>
+      </c>
       <c r="H415" s="2">
         <v>0.15920000000000001</v>
+      </c>
+      <c r="I415" s="2">
+        <v>3.5449999999999999</v>
       </c>
       <c r="J415" s="2">
         <v>1.8899999999999997</v>
@@ -13340,8 +13511,14 @@
       <c r="F416" s="2">
         <v>8.9870000000000001</v>
       </c>
+      <c r="G416" s="2">
+        <v>1.1900000000000001E-2</v>
+      </c>
       <c r="H416" s="2">
         <v>0.13470000000000001</v>
+      </c>
+      <c r="I416" s="2">
+        <v>3.2317391304347831</v>
       </c>
       <c r="J416" s="2">
         <v>1.6799999999999997</v>
@@ -13366,8 +13543,14 @@
       <c r="F417" s="2">
         <v>5.91</v>
       </c>
+      <c r="G417" s="2">
+        <v>1.1599999999999999E-2</v>
+      </c>
       <c r="H417" s="2">
         <v>0.22160000000000002</v>
+      </c>
+      <c r="I417" s="2">
+        <v>3.4157142857142859</v>
       </c>
       <c r="J417" s="2">
         <v>1.3200000000000003</v>
@@ -13392,8 +13575,14 @@
       <c r="F418" s="2">
         <v>5.1899999999999995</v>
       </c>
+      <c r="G418" s="2">
+        <v>7.899999999999999E-3</v>
+      </c>
       <c r="H418" s="2">
         <v>0.13869999999999999</v>
+      </c>
+      <c r="I418" s="2">
+        <v>3.129545454545454</v>
       </c>
       <c r="J418" s="2">
         <v>1.1799999999999997</v>
@@ -13418,8 +13607,14 @@
       <c r="F419" s="2">
         <v>-3.6869999999999998</v>
       </c>
+      <c r="G419" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
       <c r="H419" s="2">
         <v>0.11750000000000001</v>
+      </c>
+      <c r="I419" s="2">
+        <v>3.1627272727272731</v>
       </c>
       <c r="J419" s="2">
         <v>1.1399999999999997</v>
@@ -13444,8 +13639,14 @@
       <c r="F420" s="2">
         <v>5.5490000000000004</v>
       </c>
+      <c r="G420" s="2">
+        <v>3.9999999999999996E-4</v>
+      </c>
       <c r="H420" s="2">
         <v>0.248</v>
+      </c>
+      <c r="I420" s="2">
+        <v>3.031428571428572</v>
       </c>
       <c r="J420" s="2">
         <v>1.1299999999999999</v>
@@ -13470,8 +13671,14 @@
       <c r="F421" s="2">
         <v>3.2400000000000007</v>
       </c>
+      <c r="G421" s="2">
+        <v>6.2000000000000006E-3</v>
+      </c>
       <c r="H421" s="2">
         <v>0.1542</v>
+      </c>
+      <c r="I421" s="2">
+        <v>3.381739130434783</v>
       </c>
       <c r="J421" s="2">
         <v>1.1100000000000003</v>
@@ -13496,8 +13703,14 @@
       <c r="F422" s="2">
         <v>-3.4260000000000006</v>
       </c>
+      <c r="G422" s="2">
+        <v>2.8E-3</v>
+      </c>
       <c r="H422" s="2">
         <v>0.1</v>
+      </c>
+      <c r="I422" s="2">
+        <v>3.3219047619047619</v>
       </c>
       <c r="J422" s="2">
         <v>0.99000000000000021</v>
@@ -13522,8 +13735,14 @@
       <c r="F423" s="2">
         <v>3.8760000000000003</v>
       </c>
+      <c r="G423" s="2">
+        <v>1E-3</v>
+      </c>
       <c r="H423" s="2">
         <v>0.2195</v>
+      </c>
+      <c r="I423" s="2">
+        <v>3.403</v>
       </c>
       <c r="J423" s="2">
         <v>0.99000000000000021</v>
@@ -13548,8 +13767,14 @@
       <c r="F424" s="2">
         <v>6.9</v>
       </c>
+      <c r="G424" s="2">
+        <v>6.7999999999999996E-3</v>
+      </c>
       <c r="H424" s="2">
         <v>0.14450000000000002</v>
+      </c>
+      <c r="I424" s="2">
+        <v>3.5769565217391301</v>
       </c>
       <c r="J424" s="2">
         <v>1</v>
@@ -13574,8 +13799,14 @@
       <c r="F425" s="2">
         <v>2.665</v>
       </c>
+      <c r="G425" s="2">
+        <v>1.11E-2</v>
+      </c>
       <c r="H425" s="2">
         <v>9.9099999999999994E-2</v>
+      </c>
+      <c r="I425" s="2">
+        <v>3.684545454545455</v>
       </c>
       <c r="J425" s="2">
         <v>0.96</v>
@@ -13600,8 +13831,14 @@
       <c r="F426" s="2">
         <v>-8.07</v>
       </c>
+      <c r="G426" s="2">
+        <v>1.12E-2</v>
+      </c>
       <c r="H426" s="2">
         <v>0.20019999999999999</v>
+      </c>
+      <c r="I426" s="2">
+        <v>3.1047619047619048</v>
       </c>
       <c r="J426" s="2">
         <v>1.0899999999999999</v>
@@ -13626,8 +13863,14 @@
       <c r="F427" s="2">
         <v>-6.19</v>
       </c>
+      <c r="G427" s="2">
+        <v>1.2699999999999999E-2</v>
+      </c>
       <c r="H427" s="2">
         <v>0.13929999999999998</v>
+      </c>
+      <c r="I427" s="2">
+        <v>3.0804545454545451</v>
       </c>
       <c r="J427" s="2">
         <v>1.3500000000000005</v>
@@ -13652,8 +13895,14 @@
       <c r="F428" s="2">
         <v>7.4030000000000005</v>
       </c>
+      <c r="G428" s="2">
+        <v>1.4200000000000001E-2</v>
+      </c>
       <c r="H428" s="2">
         <v>0.12279999999999999</v>
+      </c>
+      <c r="I428" s="2">
+        <v>2.7240909090909091</v>
       </c>
       <c r="J428" s="2">
         <v>1.29</v>
@@ -13678,8 +13927,14 @@
       <c r="F429" s="2">
         <v>-4.7139999999999995</v>
       </c>
+      <c r="G429" s="2">
+        <v>1.26E-2</v>
+      </c>
       <c r="H429" s="2">
         <v>0.219</v>
+      </c>
+      <c r="I429" s="2">
+        <v>2.543636363636363</v>
       </c>
       <c r="J429" s="2">
         <v>1.17</v>
@@ -13704,8 +13959,14 @@
       <c r="F430" s="2">
         <v>10.073000000000002</v>
       </c>
+      <c r="G430" s="2">
+        <v>1.2500000000000001E-2</v>
+      </c>
       <c r="H430" s="2">
         <v>0.14560000000000001</v>
+      </c>
+      <c r="I430" s="2">
+        <v>2.3822727272727269</v>
       </c>
       <c r="J430" s="2">
         <v>1.1299999999999999</v>
@@ -13730,8 +13991,14 @@
       <c r="F431" s="2">
         <v>3.8249999999999993</v>
       </c>
+      <c r="G431" s="2">
+        <v>1.12E-2</v>
+      </c>
       <c r="H431" s="2">
         <v>0.1537</v>
+      </c>
+      <c r="I431" s="2">
+        <v>2.2909523809523811</v>
       </c>
       <c r="J431" s="2">
         <v>1.04</v>
@@ -13756,8 +14023,14 @@
       <c r="F432" s="2">
         <v>0.87899999999999989</v>
       </c>
+      <c r="G432" s="2">
+        <v>1.14E-2</v>
+      </c>
       <c r="H432" s="2">
         <v>0.2303</v>
+      </c>
+      <c r="I432" s="2">
+        <v>2.3818181818181818</v>
       </c>
       <c r="J432" s="2">
         <v>1.0499999999999998</v>
@@ -13782,8 +14055,14 @@
       <c r="F433" s="2">
         <v>7.0279999999999987</v>
       </c>
+      <c r="G433" s="2">
+        <v>1.3999999999999999E-2</v>
+      </c>
       <c r="H433" s="2">
         <v>0.17979999999999999</v>
+      </c>
+      <c r="I433" s="2">
+        <v>3.0130434782608688</v>
       </c>
       <c r="J433" s="2">
         <v>1.08</v>
@@ -13808,8 +14087,14 @@
       <c r="F434" s="2">
         <v>1.8039999999999998</v>
       </c>
+      <c r="G434" s="2">
+        <v>6.6000000000000008E-3</v>
+      </c>
       <c r="H434" s="2">
         <v>9.5500000000000002E-2</v>
+      </c>
+      <c r="I434" s="2">
+        <v>3.0876190476190479</v>
       </c>
       <c r="J434" s="2">
         <v>1.0499999999999998</v>
@@ -13834,8 +14119,14 @@
       <c r="F435" s="2">
         <v>3.54</v>
       </c>
+      <c r="G435" s="2">
+        <v>1.2199999999999999E-2</v>
+      </c>
       <c r="H435" s="2">
         <v>0.20409999999999998</v>
+      </c>
+      <c r="I435" s="2">
+        <v>3.2719999999999998</v>
       </c>
       <c r="J435" s="2">
         <v>0.9300000000000006</v>
@@ -13860,8 +14151,14 @@
       <c r="F436" s="2">
         <v>0.49099999999999999</v>
       </c>
+      <c r="G436" s="2">
+        <v>6.7000000000000002E-3</v>
+      </c>
       <c r="H436" s="2">
         <v>0.13550000000000001</v>
+      </c>
+      <c r="I436" s="2">
+        <v>3.3139130434782609</v>
       </c>
       <c r="J436" s="2">
         <v>0.90000000000000036</v>
@@ -13886,8 +14183,14 @@
       <c r="F437" s="2">
         <v>2.7159999999999997</v>
       </c>
+      <c r="G437" s="2">
+        <v>5.3E-3</v>
+      </c>
       <c r="H437" s="2">
         <v>0.1013</v>
+      </c>
+      <c r="I437" s="2">
+        <v>3.2347619047619052</v>
       </c>
       <c r="J437" s="2">
         <v>0.85999999999999943</v>
@@ -13912,8 +14215,14 @@
       <c r="F438" s="2">
         <v>-1.498</v>
       </c>
+      <c r="G438" s="2">
+        <v>1.2999999999999999E-3</v>
+      </c>
       <c r="H438" s="2">
         <v>0.20149999999999998</v>
+      </c>
+      <c r="I438" s="2">
+        <v>2.9854545454545458</v>
       </c>
       <c r="J438" s="2">
         <v>0.82000000000000028</v>
@@ -13938,8 +14247,14 @@
       <c r="F439" s="2">
         <v>-1.8510000000000004</v>
       </c>
+      <c r="G439" s="2">
+        <v>3.4999999999999996E-3</v>
+      </c>
       <c r="H439" s="2">
         <v>0.1343</v>
+      </c>
+      <c r="I439" s="2">
+        <v>2.9649999999999999</v>
       </c>
       <c r="J439" s="2">
         <v>0.75999999999999979</v>
@@ -13964,8 +14279,14 @@
       <c r="F440" s="2">
         <v>-2.4650000000000007</v>
       </c>
+      <c r="G440" s="2">
+        <v>-2.8E-3</v>
+      </c>
       <c r="H440" s="2">
         <v>0.10970000000000001</v>
+      </c>
+      <c r="I440" s="2">
+        <v>2.8242857142857138</v>
       </c>
       <c r="J440" s="2">
         <v>0.83000000000000007</v>
@@ -13990,8 +14311,14 @@
       <c r="F441" s="2">
         <v>-6.6960000000000006</v>
       </c>
+      <c r="G441" s="2">
+        <v>8.3000000000000001E-3</v>
+      </c>
       <c r="H441" s="2">
         <v>0.22190000000000001</v>
+      </c>
+      <c r="I441" s="2">
+        <v>2.278695652173913</v>
       </c>
       <c r="J441" s="2">
         <v>0.99000000000000021</v>
@@ -14016,8 +14343,14 @@
       <c r="F442" s="2">
         <v>-8.4160000000000004</v>
       </c>
+      <c r="G442" s="2">
+        <v>-9.9999999999999991E-5</v>
+      </c>
       <c r="H442" s="2">
         <v>0.13159999999999999</v>
+      </c>
+      <c r="I442" s="2">
+        <v>1.8722727272727271</v>
       </c>
       <c r="J442" s="2">
         <v>1.1799999999999997</v>
@@ -14042,8 +14375,14 @@
       <c r="F443" s="2">
         <v>12.315000000000001</v>
       </c>
+      <c r="G443" s="2">
+        <v>1.4E-3</v>
+      </c>
       <c r="H443" s="2">
         <v>0.13569999999999999</v>
+      </c>
+      <c r="I443" s="2">
+        <v>2.031428571428572</v>
       </c>
       <c r="J443" s="2">
         <v>1.3900000000000001</v>
@@ -14068,8 +14407,14 @@
       <c r="F444" s="2">
         <v>-1.1100000000000001</v>
       </c>
+      <c r="G444" s="2">
+        <v>3.9999999999999996E-4</v>
+      </c>
       <c r="H444" s="2">
         <v>0.26640000000000003</v>
+      </c>
+      <c r="I444" s="2">
+        <v>1.8177272727272731</v>
       </c>
       <c r="J444" s="2">
         <v>1.2699999999999996</v>
@@ -14094,8 +14439,14 @@
       <c r="F445" s="2">
         <v>-7.1999999999999981E-2</v>
       </c>
+      <c r="G445" s="2">
+        <v>0</v>
+      </c>
       <c r="H445" s="2">
         <v>0.15839999999999999</v>
+      </c>
+      <c r="I445" s="2">
+        <v>1.877272727272727</v>
       </c>
       <c r="J445" s="2">
         <v>1.3199999999999998</v>
@@ -14120,8 +14471,14 @@
       <c r="F446" s="2">
         <v>7.0830000000000002</v>
       </c>
+      <c r="G446" s="2">
+        <v>-1.9999999999999998E-4</v>
+      </c>
       <c r="H446" s="2">
         <v>0.11329999999999998</v>
+      </c>
+      <c r="I446" s="2">
+        <v>1.7563636363636359</v>
       </c>
       <c r="J446" s="2">
         <v>1.3800000000000003</v>
@@ -14146,8 +14503,14 @@
       <c r="F447" s="2">
         <v>4.649</v>
       </c>
+      <c r="G447" s="2">
+        <v>3.1000000000000003E-3</v>
+      </c>
       <c r="H447" s="2">
         <v>0.24249999999999999</v>
+      </c>
+      <c r="I447" s="2">
+        <v>1.7861904761904761</v>
       </c>
       <c r="J447" s="2">
         <v>1.2899999999999996</v>
@@ -14172,8 +14535,14 @@
       <c r="F448" s="2">
         <v>3.0390000000000006</v>
       </c>
+      <c r="G448" s="2">
+        <v>4.5999999999999999E-3</v>
+      </c>
       <c r="H448" s="2">
         <v>0.15479999999999999</v>
+      </c>
+      <c r="I448" s="2">
+        <v>2.0886363636363638</v>
       </c>
       <c r="J448" s="2">
         <v>1.2400000000000002</v>
@@ -14198,8 +14567,14 @@
       <c r="F449" s="2">
         <v>-1.81</v>
       </c>
+      <c r="G449" s="2">
+        <v>2.8999999999999998E-3</v>
+      </c>
       <c r="H449" s="2">
         <v>0.11349999999999999</v>
+      </c>
+      <c r="I449" s="2">
+        <v>1.9690476190476189</v>
       </c>
       <c r="J449" s="2">
         <v>1.2300000000000004</v>
@@ -14224,8 +14599,14 @@
       <c r="F450" s="2">
         <v>-7.5469999999999997</v>
       </c>
+      <c r="G450" s="2">
+        <v>6.4999999999999997E-3</v>
+      </c>
       <c r="H450" s="2">
         <v>0.24719999999999998</v>
+      </c>
+      <c r="I450" s="2">
+        <v>1.639130434782609</v>
       </c>
       <c r="J450" s="2">
         <v>1.2700000000000005</v>
@@ -14250,8 +14631,14 @@
       <c r="F451" s="2">
         <v>3.8860000000000001</v>
       </c>
+      <c r="G451" s="2">
+        <v>2.2000000000000001E-3</v>
+      </c>
       <c r="H451" s="2">
         <v>0.15460000000000002</v>
+      </c>
+      <c r="I451" s="2">
+        <v>1.5309523809523811</v>
       </c>
       <c r="J451" s="2">
         <v>1.3799999999999994</v>
@@ -14276,8 +14663,14 @@
       <c r="F452" s="2">
         <v>0.15899999999999992</v>
       </c>
+      <c r="G452" s="2">
+        <v>3.1999999999999997E-3</v>
+      </c>
       <c r="H452" s="2">
         <v>0.1201</v>
+      </c>
+      <c r="I452" s="2">
+        <v>1.3645454545454549</v>
       </c>
       <c r="J452" s="2">
         <v>1.4700000000000002</v>
@@ -14302,8 +14695,14 @@
       <c r="F453" s="2">
         <v>3.1590000000000003</v>
       </c>
+      <c r="G453" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
       <c r="H453" s="2">
         <v>0.26740000000000003</v>
+      </c>
+      <c r="I453" s="2">
+        <v>1.5756521739130429</v>
       </c>
       <c r="J453" s="2">
         <v>1.4300000000000002</v>
@@ -14328,8 +14727,14 @@
       <c r="F454" s="2">
         <v>2.9089999999999998</v>
       </c>
+      <c r="G454" s="2">
+        <v>6.7000000000000002E-3</v>
+      </c>
       <c r="H454" s="2">
         <v>0.14829999999999999</v>
+      </c>
+      <c r="I454" s="2">
+        <v>1.5369999999999999</v>
       </c>
       <c r="J454" s="2">
         <v>1.3499999999999996</v>
@@ -14354,8 +14759,14 @@
       <c r="F455" s="2">
         <v>-1.9200000000000004</v>
       </c>
+      <c r="G455" s="2">
+        <v>3.6999999999999997E-3</v>
+      </c>
       <c r="H455" s="2">
         <v>0.14410000000000001</v>
+      </c>
+      <c r="I455" s="2">
+        <v>1.498695652173913</v>
       </c>
       <c r="J455" s="2">
         <v>1.1099999999999999</v>
@@ -14380,8 +14791,14 @@
       <c r="F456" s="2">
         <v>0.52400000000000002</v>
       </c>
+      <c r="G456" s="2">
+        <v>8.5000000000000006E-3</v>
+      </c>
       <c r="H456" s="2">
         <v>0.31029999999999996</v>
+      </c>
+      <c r="I456" s="2">
+        <v>1.418636363636363</v>
       </c>
       <c r="J456" s="2">
         <v>1.0099999999999998</v>
@@ -14406,8 +14823,14 @@
       <c r="F457" s="2">
         <v>2.0270000000000001</v>
       </c>
+      <c r="G457" s="2">
+        <v>1.03E-2</v>
+      </c>
       <c r="H457" s="2">
         <v>0.29380000000000001</v>
+      </c>
+      <c r="I457" s="2">
+        <v>1.5704761904761899</v>
       </c>
       <c r="J457" s="2">
         <v>0.98</v>
@@ -14432,8 +14855,14 @@
       <c r="F458" s="2">
         <v>5.9789999999999992</v>
       </c>
+      <c r="G458" s="2">
+        <v>2.2000000000000001E-3</v>
+      </c>
       <c r="H458" s="2">
         <v>0.12589999999999998</v>
+      </c>
+      <c r="I458" s="2">
+        <v>1.6804347826086961</v>
       </c>
       <c r="J458" s="2">
         <v>0.9300000000000006</v>
@@ -14458,8 +14887,14 @@
       <c r="F459" s="2">
         <v>1.016</v>
       </c>
+      <c r="G459" s="2">
+        <v>5.3999999999999994E-3</v>
+      </c>
       <c r="H459" s="2">
         <v>0.23649999999999999</v>
+      </c>
+      <c r="I459" s="2">
+        <v>1.7909999999999999</v>
       </c>
       <c r="J459" s="2">
         <v>0.94999999999999973</v>
@@ -14484,8 +14919,14 @@
       <c r="F460" s="2">
         <v>4.3449999999999998</v>
       </c>
+      <c r="G460" s="2">
+        <v>4.1000000000000003E-3</v>
+      </c>
       <c r="H460" s="2">
         <v>0.13789999999999999</v>
+      </c>
+      <c r="I460" s="2">
+        <v>1.7814285714285709</v>
       </c>
       <c r="J460" s="2">
         <v>0.91999999999999948</v>
@@ -14510,8 +14951,14 @@
       <c r="F461" s="2">
         <v>1.419</v>
       </c>
+      <c r="G461" s="2">
+        <v>3.6999999999999997E-3</v>
+      </c>
       <c r="H461" s="2">
         <v>0.1048</v>
+      </c>
+      <c r="I461" s="2">
+        <v>1.699090909090909</v>
       </c>
       <c r="J461" s="2">
         <v>0.85999999999999988</v>
@@ -14536,8 +14983,14 @@
       <c r="F462" s="2">
         <v>3.1149999999999998</v>
       </c>
+      <c r="G462" s="2">
+        <v>1.2000000000000001E-3</v>
+      </c>
       <c r="H462" s="2">
         <v>0.26489999999999997</v>
+      </c>
+      <c r="I462" s="2">
+        <v>1.802173913043478</v>
       </c>
       <c r="J462" s="2">
         <v>0.8400000000000003</v>
@@ -14562,8 +15015,14 @@
       <c r="F463" s="2">
         <v>-1.768</v>
       </c>
+      <c r="G463" s="2">
+        <v>1.2999999999999999E-3</v>
+      </c>
       <c r="H463" s="2">
         <v>0.14580000000000001</v>
+      </c>
+      <c r="I463" s="2">
+        <v>2.2494999999999998</v>
       </c>
       <c r="J463" s="2">
         <v>0.92000000000000082</v>
@@ -14588,8 +15047,14 @@
       <c r="F464" s="2">
         <v>6.3239999999999998</v>
       </c>
+      <c r="G464" s="2">
+        <v>8.9999999999999998E-4</v>
+      </c>
       <c r="H464" s="2">
         <v>0.1394</v>
+      </c>
+      <c r="I464" s="2">
+        <v>2.4360869565217391</v>
       </c>
       <c r="J464" s="2">
         <v>0.98000000000000043</v>
@@ -14614,8 +15079,14 @@
       <c r="F465" s="2">
         <v>-2.4209999999999998</v>
       </c>
+      <c r="G465" s="2">
+        <v>8.9999999999999998E-4</v>
+      </c>
       <c r="H465" s="2">
         <v>0.22599999999999998</v>
+      </c>
+      <c r="I465" s="2">
+        <v>2.6936363636363629</v>
       </c>
       <c r="J465" s="2">
         <v>0.87999999999999989</v>
@@ -14640,8 +15111,14 @@
       <c r="F466" s="2">
         <v>3.9880000000000004</v>
       </c>
+      <c r="G466" s="2">
+        <v>7.9999999999999993E-4</v>
+      </c>
       <c r="H466" s="2">
         <v>0.1371</v>
+      </c>
+      <c r="I466" s="2">
+        <v>2.66047619047619</v>
       </c>
       <c r="J466" s="2">
         <v>0.83000000000000007</v>
@@ -14666,8 +15143,14 @@
       <c r="F467" s="2">
         <v>4.0709999999999997</v>
       </c>
+      <c r="G467" s="2">
+        <v>1.6999999999999999E-3</v>
+      </c>
       <c r="H467" s="2">
         <v>0.1207</v>
+      </c>
+      <c r="I467" s="2">
+        <v>2.45695652173913</v>
       </c>
       <c r="J467" s="2">
         <v>0.77999999999999936</v>
@@ -14692,8 +15175,14 @@
       <c r="F468" s="2">
         <v>3.1640000000000001</v>
       </c>
+      <c r="G468" s="2">
+        <v>3.1999999999999997E-3</v>
+      </c>
       <c r="H468" s="2">
         <v>0.22509999999999999</v>
+      </c>
+      <c r="I468" s="2">
+        <v>2.3980952380952378</v>
       </c>
       <c r="J468" s="2">
         <v>0.75</v>
@@ -14718,8 +15207,14 @@
       <c r="F469" s="2">
         <v>2.625</v>
       </c>
+      <c r="G469" s="2">
+        <v>2.3E-3</v>
+      </c>
       <c r="H469" s="2">
         <v>0.14959999999999998</v>
+      </c>
+      <c r="I469" s="2">
+        <v>2.706363636363637</v>
       </c>
       <c r="J469" s="2">
         <v>0.75999999999999979</v>
@@ -14744,8 +15239,14 @@
       <c r="F470" s="2">
         <v>-3.117</v>
       </c>
+      <c r="G470" s="2">
+        <v>1.2000000000000001E-3</v>
+      </c>
       <c r="H470" s="2">
         <v>0.10690000000000001</v>
+      </c>
+      <c r="I470" s="2">
+        <v>2.57</v>
       </c>
       <c r="J470" s="2">
         <v>0.70000000000000018</v>
@@ -14770,8 +15271,14 @@
       <c r="F471" s="2">
         <v>4.8609999999999998</v>
       </c>
+      <c r="G471" s="2">
+        <v>4.5000000000000005E-3</v>
+      </c>
       <c r="H471" s="2">
         <v>0.23649999999999999</v>
+      </c>
+      <c r="I471" s="2">
+        <v>2.524</v>
       </c>
       <c r="J471" s="2">
         <v>0.64999999999999947</v>
@@ -14796,8 +15303,14 @@
       <c r="F472" s="2">
         <v>0.40200000000000002</v>
       </c>
+      <c r="G472" s="2">
+        <v>2.8E-3</v>
+      </c>
       <c r="H472" s="2">
         <v>0.1331</v>
+      </c>
+      <c r="I472" s="2">
+        <v>2.670952380952381</v>
       </c>
       <c r="J472" s="2">
         <v>0.67999999999999972</v>
@@ -14822,8 +15335,14 @@
       <c r="F473" s="2">
         <v>-7.0000000000000104E-2</v>
       </c>
+      <c r="G473" s="2">
+        <v>1.5E-3</v>
+      </c>
       <c r="H473" s="2">
         <v>0.107</v>
+      </c>
+      <c r="I473" s="2">
+        <v>2.5527272727272732</v>
       </c>
       <c r="J473" s="2">
         <v>0.66000000000000014</v>
@@ -14848,8 +15367,14 @@
       <c r="F474" s="2">
         <v>2.097</v>
       </c>
+      <c r="G474" s="2">
+        <v>7.9999999999999993E-4</v>
+      </c>
       <c r="H474" s="2">
         <v>0.22520000000000001</v>
+      </c>
+      <c r="I474" s="2">
+        <v>2.4118181818181821</v>
       </c>
       <c r="J474" s="2">
         <v>0.59999999999999964</v>
@@ -14874,8 +15399,14 @@
       <c r="F475" s="2">
         <v>2.9880000000000004</v>
       </c>
+      <c r="G475" s="2">
+        <v>2E-3</v>
+      </c>
       <c r="H475" s="2">
         <v>0.14220000000000002</v>
+      </c>
+      <c r="I475" s="2">
+        <v>2.5628571428571432</v>
       </c>
       <c r="J475" s="2">
         <v>0.54999999999999982</v>
@@ -14900,8 +15431,14 @@
       <c r="F476" s="2">
         <v>-1.9809999999999999</v>
       </c>
+      <c r="G476" s="2">
+        <v>1.2999999999999999E-3</v>
+      </c>
       <c r="H476" s="2">
         <v>0.12819999999999998</v>
+      </c>
+      <c r="I476" s="2">
+        <v>2.4065217391304352</v>
       </c>
       <c r="J476" s="2">
         <v>0.57000000000000028</v>
@@ -14926,8 +15463,14 @@
       <c r="F477" s="2">
         <v>4.3580000000000005</v>
       </c>
+      <c r="G477" s="2">
+        <v>3.0000000000000003E-4</v>
+      </c>
       <c r="H477" s="2">
         <v>0.20980000000000001</v>
+      </c>
+      <c r="I477" s="2">
+        <v>2.387142857142857</v>
       </c>
       <c r="J477" s="2">
         <v>0.61000000000000032</v>
@@ -14952,8 +15495,14 @@
       <c r="F478" s="2">
         <v>-2.4889999999999999</v>
       </c>
+      <c r="G478" s="2">
+        <v>3.9999999999999996E-4</v>
+      </c>
       <c r="H478" s="2">
         <v>0.13290000000000002</v>
+      </c>
+      <c r="I478" s="2">
+        <v>2.4</v>
       </c>
       <c r="J478" s="2">
         <v>0.6899999999999995</v>
@@ -14978,8 +15527,14 @@
       <c r="F479" s="2">
         <v>2.5089999999999995</v>
       </c>
+      <c r="G479" s="2">
+        <v>1.2000000000000001E-3</v>
+      </c>
       <c r="H479" s="2">
         <v>0.11789999999999999</v>
+      </c>
+      <c r="I479" s="2">
+        <v>2.1878260869565218</v>
       </c>
       <c r="J479" s="2">
         <v>0.77000000000000046</v>
@@ -15004,8 +15559,14 @@
       <c r="F480" s="2">
         <v>2.048</v>
       </c>
+      <c r="G480" s="2">
+        <v>-9.9999999999999991E-5</v>
+      </c>
       <c r="H480" s="2">
         <v>0.23100000000000001</v>
+      </c>
+      <c r="I480" s="2">
+        <v>2.0735000000000001</v>
       </c>
       <c r="J480" s="2">
         <v>0.87000000000000011</v>
@@ -15030,8 +15591,14 @@
       <c r="F481" s="2">
         <v>-0.27600000000000002</v>
       </c>
+      <c r="G481" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="H481" s="2">
         <v>0.14809999999999998</v>
+      </c>
+      <c r="I481" s="2">
+        <v>2.083478260869565</v>
       </c>
       <c r="J481" s="2">
         <v>0.95000000000000018</v>
@@ -15056,8 +15623,14 @@
       <c r="F482" s="2">
         <v>-3.9389999999999992</v>
       </c>
+      <c r="G482" s="2">
+        <v>1.2999999999999999E-3</v>
+      </c>
       <c r="H482" s="2">
         <v>0.10709999999999999</v>
+      </c>
+      <c r="I482" s="2">
+        <v>1.6854545454545451</v>
       </c>
       <c r="J482" s="2">
         <v>0.99000000000000021</v>
@@ -15082,8 +15655,14 @@
       <c r="F483" s="2">
         <v>6.8809999999999985</v>
       </c>
+      <c r="G483" s="2">
+        <v>-2.0999999999999999E-3</v>
+      </c>
       <c r="H483" s="2">
         <v>0.251</v>
+      </c>
+      <c r="I483" s="2">
+        <v>1.8594999999999999</v>
       </c>
       <c r="J483" s="2">
         <v>0.89999999999999991</v>
@@ -15108,8 +15687,14 @@
       <c r="F484" s="2">
         <v>-1.5870000000000002</v>
       </c>
+      <c r="G484" s="2">
+        <v>-7.9999999999999993E-4</v>
+      </c>
       <c r="H484" s="2">
         <v>0.14760000000000001</v>
+      </c>
+      <c r="I484" s="2">
+        <v>2.0150000000000001</v>
       </c>
       <c r="J484" s="2">
         <v>0.89999999999999991</v>
@@ -15134,8 +15719,14 @@
       <c r="F485" s="2">
         <v>2.2950000000000004</v>
       </c>
+      <c r="G485" s="2">
+        <v>2.8999999999999998E-3</v>
+      </c>
       <c r="H485" s="2">
         <v>0.1023</v>
+      </c>
+      <c r="I485" s="2">
+        <v>1.9118181818181821</v>
       </c>
       <c r="J485" s="2">
         <v>0.96000000000000041</v>
@@ -15160,8 +15751,14 @@
       <c r="F486" s="2">
         <v>0.1410000000000001</v>
       </c>
+      <c r="G486" s="2">
+        <v>-5.0000000000000001E-4</v>
+      </c>
       <c r="H486" s="2">
         <v>0.22360000000000002</v>
+      </c>
+      <c r="I486" s="2">
+        <v>2.077142857142857</v>
       </c>
       <c r="J486" s="2">
         <v>0.9099999999999997</v>
@@ -15186,8 +15783,14 @@
       <c r="F487" s="2">
         <v>-2.0529999999999999</v>
       </c>
+      <c r="G487" s="2">
+        <v>3.9999999999999996E-4</v>
+      </c>
       <c r="H487" s="2">
         <v>0.14019999999999999</v>
+      </c>
+      <c r="I487" s="2">
+        <v>2.3486363636363641</v>
       </c>
       <c r="J487" s="2">
         <v>0.9399999999999995</v>
@@ -15212,8 +15815,14 @@
       <c r="F488" s="2">
         <v>-1.1559999999999997</v>
       </c>
+      <c r="G488" s="2">
+        <v>-3.6999999999999997E-3</v>
+      </c>
       <c r="H488" s="2">
         <v>0.11650000000000001</v>
+      </c>
+      <c r="I488" s="2">
+        <v>2.192608695652174</v>
       </c>
       <c r="J488" s="2">
         <v>1.0499999999999998</v>
@@ -15238,8 +15847,14 @@
       <c r="F489" s="2">
         <v>-5.6769999999999996</v>
       </c>
+      <c r="G489" s="2">
+        <v>2.6999999999999997E-3</v>
+      </c>
       <c r="H489" s="2">
         <v>0.21920000000000001</v>
+      </c>
+      <c r="I489" s="2">
+        <v>2.0952380952380949</v>
       </c>
       <c r="J489" s="2">
         <v>1.1500000000000004</v>
@@ -15264,8 +15879,14 @@
       <c r="F490" s="2">
         <v>-4.5909999999999993</v>
       </c>
+      <c r="G490" s="2">
+        <v>-6.0000000000000006E-4</v>
+      </c>
       <c r="H490" s="2">
         <v>0.14610000000000001</v>
+      </c>
+      <c r="I490" s="2">
+        <v>2.0527272727272732</v>
       </c>
       <c r="J490" s="2">
         <v>1.2699999999999996</v>
@@ -15290,8 +15911,14 @@
       <c r="F491" s="2">
         <v>8.1699999999999982</v>
       </c>
+      <c r="G491" s="2">
+        <v>-2.6999999999999997E-3</v>
+      </c>
       <c r="H491" s="2">
         <v>0.13170000000000001</v>
+      </c>
+      <c r="I491" s="2">
+        <v>1.961363636363636</v>
       </c>
       <c r="J491" s="2">
         <v>1.3899999999999997</v>
@@ -15316,8 +15943,14 @@
       <c r="F492" s="2">
         <v>-3.299999999999996E-2</v>
       </c>
+      <c r="G492" s="2">
+        <v>2E-3</v>
+      </c>
       <c r="H492" s="2">
         <v>0.23939999999999997</v>
+      </c>
+      <c r="I492" s="2">
+        <v>1.9347619047619049</v>
       </c>
       <c r="J492" s="2">
         <v>1.4000000000000004</v>
@@ -15342,8 +15975,14 @@
       <c r="F493" s="2">
         <v>-2.8420000000000001</v>
       </c>
+      <c r="G493" s="2">
+        <v>1.03E-2</v>
+      </c>
       <c r="H493" s="2">
         <v>0.16119999999999998</v>
+      </c>
+      <c r="I493" s="2">
+        <v>1.9273913043478259</v>
       </c>
       <c r="J493" s="2">
         <v>1.4899999999999998</v>
@@ -15368,8 +16007,14 @@
       <c r="F494" s="2">
         <v>-6.5140000000000002</v>
       </c>
+      <c r="G494" s="2">
+        <v>3.6999999999999997E-3</v>
+      </c>
       <c r="H494" s="2">
         <v>0.12359999999999999</v>
+      </c>
+      <c r="I494" s="2">
+        <v>1.655714285714285</v>
       </c>
       <c r="J494" s="2">
         <v>1.4500000000000002</v>
@@ -15394,8 +16039,14 @@
       <c r="F495" s="2">
         <v>0.84399999999999997</v>
       </c>
+      <c r="G495" s="2">
+        <v>2.0500000000000001E-2</v>
+      </c>
       <c r="H495" s="2">
         <v>0.26369999999999999</v>
+      </c>
+      <c r="I495" s="2">
+        <v>1.397142857142857</v>
       </c>
       <c r="J495" s="2">
         <v>1.38</v>
@@ -15420,8 +16071,14 @@
       <c r="F496" s="2">
         <v>8.0389999999999997</v>
       </c>
+      <c r="G496" s="2">
+        <v>1.9E-2</v>
+      </c>
       <c r="H496" s="2">
         <v>0.18090000000000001</v>
+      </c>
+      <c r="I496" s="2">
+        <v>1.5256521739130431</v>
       </c>
       <c r="J496" s="2">
         <v>1.31</v>
@@ -15446,8 +16103,14 @@
       <c r="F497" s="2">
         <v>3.5229999999999997</v>
       </c>
+      <c r="G497" s="2">
+        <v>5.1000000000000004E-3</v>
+      </c>
       <c r="H497" s="2">
         <v>0.11460000000000001</v>
+      </c>
+      <c r="I497" s="2">
+        <v>1.577142857142857</v>
       </c>
       <c r="J497" s="2">
         <v>1.17</v>
@@ -15472,8 +16135,14 @@
       <c r="F498" s="2">
         <v>1.296</v>
       </c>
+      <c r="G498" s="2">
+        <v>1.15E-2</v>
+      </c>
       <c r="H498" s="2">
         <v>0.24629999999999999</v>
+      </c>
+      <c r="I498" s="2">
+        <v>1.4622727272727269</v>
       </c>
       <c r="J498" s="2">
         <v>1.0299999999999998</v>
@@ -15498,8 +16167,14 @@
       <c r="F499" s="2">
         <v>-0.71399999999999975</v>
       </c>
+      <c r="G499" s="2">
+        <v>1.8799999999999997E-2</v>
+      </c>
       <c r="H499" s="2">
         <v>0.1487</v>
+      </c>
+      <c r="I499" s="2">
+        <v>1.374545454545455</v>
       </c>
       <c r="J499" s="2">
         <v>1.0300000000000002</v>
@@ -15524,8 +16199,14 @@
       <c r="F500" s="2">
         <v>5.0960000000000001</v>
       </c>
+      <c r="G500" s="2">
+        <v>1.7100000000000001E-2</v>
+      </c>
       <c r="H500" s="2">
         <v>0.12210000000000001</v>
+      </c>
+      <c r="I500" s="2">
+        <v>1.1490476190476191</v>
       </c>
       <c r="J500" s="2">
         <v>0.94</v>
@@ -15550,8 +16231,14 @@
       <c r="F501" s="2">
         <v>1.1870000000000001</v>
       </c>
+      <c r="G501" s="2">
+        <v>1.6500000000000001E-2</v>
+      </c>
       <c r="H501" s="2">
         <v>0.25869999999999999</v>
+      </c>
+      <c r="I501" s="2">
+        <v>1.2591304347826091</v>
       </c>
       <c r="J501" s="2">
         <v>0.92000000000000037</v>
@@ -15576,8 +16263,14 @@
       <c r="F502" s="2">
         <v>0.78900000000000003</v>
       </c>
+      <c r="G502" s="2">
+        <v>2.1900000000000003E-2</v>
+      </c>
       <c r="H502" s="2">
         <v>0.11650000000000001</v>
+      </c>
+      <c r="I502" s="2">
+        <v>1.277727272727273</v>
       </c>
       <c r="J502" s="2">
         <v>0.89999999999999947</v>
@@ -15602,8 +16295,14 @@
       <c r="F503" s="2">
         <v>-2.6919999999999997</v>
       </c>
+      <c r="G503" s="2">
+        <v>1.6799999999999999E-2</v>
+      </c>
       <c r="H503" s="2">
         <v>0.12359999999999999</v>
+      </c>
+      <c r="I503" s="2">
+        <v>1.3695238095238089</v>
       </c>
       <c r="J503" s="2">
         <v>0.87000000000000011</v>
@@ -15628,8 +16327,14 @@
       <c r="F504" s="2">
         <v>5.6550000000000002</v>
       </c>
+      <c r="G504" s="2">
+        <v>1.3599999999999999E-2</v>
+      </c>
       <c r="H504" s="2">
         <v>0.27360000000000001</v>
+      </c>
+      <c r="I504" s="2">
+        <v>1.541818181818182</v>
       </c>
       <c r="J504" s="2">
         <v>0.85000000000000009</v>
@@ -15654,8 +16359,14 @@
       <c r="F505" s="2">
         <v>1.4769999999999999</v>
       </c>
+      <c r="G505" s="2">
+        <v>2.3900000000000001E-2</v>
+      </c>
       <c r="H505" s="2">
         <v>0.13170000000000001</v>
+      </c>
+      <c r="I505" s="2">
+        <v>1.896363636363636</v>
       </c>
       <c r="J505" s="2">
         <v>0.77000000000000046</v>
@@ -15680,8 +16391,14 @@
       <c r="F506" s="2">
         <v>2.1569999999999996</v>
       </c>
+      <c r="G506" s="2">
+        <v>3.5799999999999998E-2</v>
+      </c>
       <c r="H506" s="2">
         <v>0.11119999999999999</v>
+      </c>
+      <c r="I506" s="2">
+        <v>1.7463636363636359</v>
       </c>
       <c r="J506" s="2">
         <v>0.74000000000000021</v>
@@ -15706,8 +16423,14 @@
       <c r="F507" s="2">
         <v>3.0659999999999998</v>
       </c>
+      <c r="G507" s="2">
+        <v>3.6400000000000002E-2</v>
+      </c>
       <c r="H507" s="2">
         <v>0.23430000000000001</v>
+      </c>
+      <c r="I507" s="2">
+        <v>1.8029999999999999</v>
       </c>
       <c r="J507" s="2">
         <v>0.6899999999999995</v>
@@ -15732,8 +16455,14 @@
       <c r="F508" s="2">
         <v>-4.6999999999999993E-2</v>
       </c>
+      <c r="G508" s="2">
+        <v>3.5299999999999998E-2</v>
+      </c>
       <c r="H508" s="2">
         <v>0.13999999999999999</v>
+      </c>
+      <c r="I508" s="2">
+        <v>1.744347826086956</v>
       </c>
       <c r="J508" s="2">
         <v>0.66999999999999993</v>
@@ -15758,8 +16487,14 @@
       <c r="F509" s="2">
         <v>1.0860000000000001</v>
       </c>
+      <c r="G509" s="2">
+        <v>5.3700000000000005E-2</v>
+      </c>
       <c r="H509" s="2">
         <v>0.1094</v>
+      </c>
+      <c r="I509" s="2">
+        <v>1.4239999999999999</v>
       </c>
       <c r="J509" s="2">
         <v>0.70000000000000018</v>
@@ -15784,8 +16519,14 @@
       <c r="F510" s="2">
         <v>0.58099999999999996</v>
       </c>
+      <c r="G510" s="2">
+        <v>6.1399999999999996E-2</v>
+      </c>
       <c r="H510" s="2">
         <v>0.24780000000000002</v>
+      </c>
+      <c r="I510" s="2">
+        <v>1.35304347826087</v>
       </c>
       <c r="J510" s="2">
         <v>0.69999999999999973</v>
@@ -15810,8 +16551,14 @@
       <c r="F511" s="2">
         <v>1.1059999999999999</v>
       </c>
+      <c r="G511" s="2">
+        <v>6.1700000000000005E-2</v>
+      </c>
       <c r="H511" s="2">
         <v>0.12290000000000001</v>
+      </c>
+      <c r="I511" s="2">
+        <v>1.2040909090909091</v>
       </c>
       <c r="J511" s="2">
         <v>0.69</v>
@@ -15836,8 +16583,14 @@
       <c r="F512" s="2">
         <v>1.7439999999999998</v>
       </c>
+      <c r="G512" s="2">
+        <v>7.22E-2</v>
+      </c>
       <c r="H512" s="2">
         <v>0.14510000000000001</v>
+      </c>
+      <c r="I512" s="2">
+        <v>1.1914285714285719</v>
       </c>
       <c r="J512" s="2">
         <v>0.6899999999999995</v>
@@ -15862,8 +16615,14 @@
       <c r="F513" s="2">
         <v>-0.26600000000000007</v>
       </c>
+      <c r="G513" s="2">
+        <v>8.270000000000001E-2</v>
+      </c>
       <c r="H513" s="2">
         <v>0.247</v>
+      </c>
+      <c r="I513" s="2">
+        <v>1.1947826086956519</v>
       </c>
       <c r="J513" s="2">
         <v>0.67999999999999972</v>
@@ -15888,8 +16647,14 @@
       <c r="F514" s="2">
         <v>3.1859999999999999</v>
       </c>
+      <c r="G514" s="2">
+        <v>9.4399999999999998E-2</v>
+      </c>
       <c r="H514" s="2">
         <v>0.10289999999999999</v>
+      </c>
+      <c r="I514" s="2">
+        <v>1.1166666666666669</v>
       </c>
       <c r="J514" s="2">
         <v>0.66999999999999993</v>
@@ -15914,8 +16679,14 @@
       <c r="F515" s="2">
         <v>1.1870000000000001</v>
       </c>
+      <c r="G515" s="2">
+        <v>8.4000000000000005E-2</v>
+      </c>
       <c r="H515" s="2">
         <v>0.10660000000000001</v>
+      </c>
+      <c r="I515" s="2">
+        <v>1.226818181818182</v>
       </c>
       <c r="J515" s="2">
         <v>0.7200000000000002</v>
@@ -15940,8 +16711,14 @@
       <c r="F516" s="2">
         <v>3.8689999999999998</v>
       </c>
+      <c r="G516" s="2">
+        <v>8.2600000000000007E-2</v>
+      </c>
       <c r="H516" s="2">
         <v>0.25319999999999998</v>
+      </c>
+      <c r="I516" s="2">
+        <v>1.072727272727273</v>
       </c>
       <c r="J516" s="2">
         <v>0.69999999999999973</v>
@@ -15966,8 +16743,14 @@
       <c r="F517" s="2">
         <v>1.4650000000000001</v>
       </c>
+      <c r="G517" s="2">
+        <v>8.8400000000000006E-2</v>
+      </c>
       <c r="H517" s="2">
         <v>0.1038</v>
+      </c>
+      <c r="I517" s="2">
+        <v>1.029047619047619</v>
       </c>
       <c r="J517" s="2">
         <v>0.71</v>
@@ -15992,8 +16775,14 @@
       <c r="F518" s="2">
         <v>4.6639999999999997</v>
       </c>
+      <c r="G518" s="2">
+        <v>0.11210000000000001</v>
+      </c>
       <c r="H518" s="2">
         <v>0.10300000000000001</v>
+      </c>
+      <c r="I518" s="2">
+        <v>1.068695652173913</v>
       </c>
       <c r="J518" s="2">
         <v>0.71</v>
@@ -16018,8 +16807,14 @@
       <c r="F519" s="2">
         <v>-4.3849999999999998</v>
       </c>
+      <c r="G519" s="2">
+        <v>0.10729999999999999</v>
+      </c>
       <c r="H519" s="2">
         <v>0.2049</v>
+      </c>
+      <c r="I519" s="2">
+        <v>1.2264999999999999</v>
       </c>
       <c r="J519" s="2">
         <v>0.69</v>
@@ -16044,8 +16839,14 @@
       <c r="F520" s="2">
         <v>-1.8060000000000003</v>
       </c>
+      <c r="G520" s="2">
+        <v>2.6100000000000002E-2</v>
+      </c>
       <c r="H520" s="2">
         <v>0.13979999999999998</v>
+      </c>
+      <c r="I520" s="2">
+        <v>1.093636363636364</v>
       </c>
       <c r="J520" s="2">
         <v>0.76999999999999957</v>
@@ -16070,8 +16871,14 @@
       <c r="F521" s="2">
         <v>0.55800000000000005</v>
       </c>
+      <c r="G521" s="2">
+        <v>0.14330000000000001</v>
+      </c>
       <c r="H521" s="2">
         <v>0.1046</v>
+      </c>
+      <c r="I521" s="2">
+        <v>1.111428571428571</v>
       </c>
       <c r="J521" s="2">
         <v>0.81999999999999984</v>
@@ -16096,8 +16903,14 @@
       <c r="F522" s="2">
         <v>2.3120000000000003</v>
       </c>
+      <c r="G522" s="2">
+        <v>0.1401</v>
+      </c>
       <c r="H522" s="2">
         <v>0.24299999999999999</v>
+      </c>
+      <c r="I522" s="2">
+        <v>1.0652173913043479</v>
       </c>
       <c r="J522" s="2">
         <v>0.83000000000000007</v>
@@ -16122,8 +16935,14 @@
       <c r="F523" s="2">
         <v>1.0240000000000002</v>
       </c>
+      <c r="G523" s="2">
+        <v>0.14080000000000001</v>
+      </c>
       <c r="H523" s="2">
         <v>0.1111</v>
+      </c>
+      <c r="I523" s="2">
+        <v>1.013333333333333</v>
       </c>
       <c r="J523" s="2">
         <v>0.87000000000000011</v>
@@ -16148,8 +16967,14 @@
       <c r="F524" s="2">
         <v>3.4609999999999994</v>
       </c>
+      <c r="G524" s="2">
+        <v>0.15579999999999999</v>
+      </c>
       <c r="H524" s="2">
         <v>0.11019999999999999</v>
+      </c>
+      <c r="I524" s="2">
+        <v>0.88954545454545453</v>
       </c>
       <c r="J524" s="2">
         <v>0.91999999999999993</v>
@@ -16174,8 +16999,14 @@
       <c r="F525" s="2">
         <v>3.2590000000000003</v>
       </c>
+      <c r="G525" s="2">
+        <v>0.1575</v>
+      </c>
       <c r="H525" s="2">
         <v>0.22599999999999998</v>
+      </c>
+      <c r="I525" s="2">
+        <v>0.85521739130434793</v>
       </c>
       <c r="J525" s="2">
         <v>0.88999999999999968</v>
@@ -16200,8 +17031,14 @@
       <c r="F526" s="2">
         <v>0.10099999999999998</v>
       </c>
+      <c r="G526" s="2">
+        <v>0.14899999999999999</v>
+      </c>
       <c r="H526" s="2">
         <v>0.1101</v>
+      </c>
+      <c r="I526" s="2">
+        <v>0.83399999999999996</v>
       </c>
       <c r="J526" s="2">
         <v>0.89999999999999991</v>
@@ -16226,8 +17063,14 @@
       <c r="F527" s="2">
         <v>-7.4539999999999988</v>
       </c>
+      <c r="G527" s="2">
+        <v>0.189</v>
+      </c>
       <c r="H527" s="2">
         <v>0.10389999999999999</v>
+      </c>
+      <c r="I527" s="2">
+        <v>0.86391304347826092</v>
       </c>
       <c r="J527" s="2">
         <v>0.9300000000000006</v>
@@ -16252,8 +17095,14 @@
       <c r="F528" s="2">
         <v>1.6620000000000001</v>
       </c>
+      <c r="G528" s="2">
+        <v>0.17949999999999999</v>
+      </c>
       <c r="H528" s="2">
         <v>0.24429999999999999</v>
+      </c>
+      <c r="I528" s="2">
+        <v>0.71863636363636374</v>
       </c>
       <c r="J528" s="2">
         <v>1</v>
@@ -16278,8 +17127,14 @@
       <c r="F529" s="2">
         <v>-9.93</v>
       </c>
+      <c r="G529" s="2">
+        <v>0.193</v>
+      </c>
       <c r="H529" s="2">
         <v>0.1389</v>
+      </c>
+      <c r="I529" s="2">
+        <v>0.42238095238095241</v>
       </c>
       <c r="J529" s="2">
         <v>1.1100000000000003</v>
@@ -16304,8 +17159,14 @@
       <c r="F530" s="2">
         <v>11.012</v>
       </c>
+      <c r="G530" s="2">
+        <v>0.192</v>
+      </c>
       <c r="H530" s="2">
         <v>0.13639999999999999</v>
+      </c>
+      <c r="I530" s="2">
+        <v>0.31000000000000011</v>
       </c>
       <c r="J530" s="2">
         <v>1.19</v>
@@ -16330,8 +17191,14 @@
       <c r="F531" s="2">
         <v>3.7279999999999993</v>
       </c>
+      <c r="G531" s="2">
+        <v>0.18090000000000001</v>
+      </c>
       <c r="H531" s="2">
         <v>0.22390000000000002</v>
+      </c>
+      <c r="I531" s="2">
+        <v>0.27350000000000002</v>
       </c>
       <c r="J531" s="2">
         <v>1.1600000000000001</v>
@@ -16356,8 +17223,14 @@
       <c r="F532" s="2">
         <v>0.93599999999999994</v>
       </c>
+      <c r="G532" s="2">
+        <v>0.19350000000000001</v>
+      </c>
       <c r="H532" s="2">
         <v>0.13090000000000002</v>
+      </c>
+      <c r="I532" s="2">
+        <v>0.16857142857142851</v>
       </c>
       <c r="J532" s="2">
         <v>1.0699999999999998</v>
@@ -16382,8 +17255,14 @@
       <c r="F533" s="2">
         <v>4.399</v>
       </c>
+      <c r="G533" s="2">
+        <v>0.21250000000000002</v>
+      </c>
       <c r="H533" s="2">
         <v>0.11</v>
+      </c>
+      <c r="I533" s="2">
+        <v>0.14272727272727259</v>
       </c>
       <c r="J533" s="2">
         <v>1.0100000000000002</v>
@@ -16408,8 +17287,14 @@
       <c r="F534" s="2">
         <v>-8.7680000000000007</v>
       </c>
+      <c r="G534" s="2">
+        <v>0.1983</v>
+      </c>
       <c r="H534" s="2">
         <v>0.22430000000000003</v>
+      </c>
+      <c r="I534" s="2">
+        <v>4.0434782608695763E-2</v>
       </c>
       <c r="J534" s="2">
         <v>0.96</v>
@@ -16434,8 +17319,14 @@
       <c r="F535" s="2">
         <v>7.95</v>
       </c>
+      <c r="G535" s="2">
+        <v>0.18529999999999999</v>
+      </c>
       <c r="H535" s="2">
         <v>0.12539999999999998</v>
+      </c>
+      <c r="I535" s="2">
+        <v>-9.650000000000003E-2</v>
       </c>
       <c r="J535" s="2">
         <v>1.04</v>
@@ -16460,8 +17351,14 @@
       <c r="F536" s="2">
         <v>0.71700000000000008</v>
       </c>
+      <c r="G536" s="2">
+        <v>0.17830000000000001</v>
+      </c>
       <c r="H536" s="2">
         <v>0.11889999999999999</v>
+      </c>
+      <c r="I536" s="2">
+        <v>-3.782608695652178E-2</v>
       </c>
       <c r="J536" s="2">
         <v>0.99000000000000021</v>
@@ -16486,8 +17383,14 @@
       <c r="F537" s="2">
         <v>-4.7679999999999998</v>
       </c>
+      <c r="G537" s="2">
+        <v>0.1908</v>
+      </c>
       <c r="H537" s="2">
         <v>0.2198</v>
+      </c>
+      <c r="I537" s="2">
+        <v>-0.32318181818181813</v>
       </c>
       <c r="J537" s="2">
         <v>0.89000000000000012</v>
@@ -16512,8 +17415,14 @@
       <c r="F538" s="2">
         <v>2.8199999999999994</v>
       </c>
+      <c r="G538" s="2">
+        <v>0.1787</v>
+      </c>
       <c r="H538" s="2">
         <v>0.12539999999999998</v>
+      </c>
+      <c r="I538" s="2">
+        <v>-0.18571428571428569</v>
       </c>
       <c r="J538" s="2">
         <v>0.88000000000000034</v>
@@ -16538,8 +17447,14 @@
       <c r="F539" s="2">
         <v>1.9780000000000002</v>
       </c>
+      <c r="G539" s="2">
+        <v>0.15310000000000001</v>
+      </c>
       <c r="H539" s="2">
         <v>0.1166</v>
+      </c>
+      <c r="I539" s="2">
+        <v>5.739130434782614E-2</v>
       </c>
       <c r="J539" s="2">
         <v>0.91000000000000014</v>
@@ -16564,8 +17479,14 @@
       <c r="F540" s="2">
         <v>4.4990000000000006</v>
       </c>
+      <c r="G540" s="2">
+        <v>0.11969999999999999</v>
+      </c>
       <c r="H540" s="2">
         <v>0.21920000000000001</v>
+      </c>
+      <c r="I540" s="2">
+        <v>0.24428571428571419</v>
       </c>
       <c r="J540" s="2">
         <v>0.87999999999999989</v>
@@ -16590,8 +17511,14 @@
       <c r="F541" s="2">
         <v>3.9240000000000004</v>
       </c>
+      <c r="G541" s="2">
+        <v>0.1431</v>
+      </c>
       <c r="H541" s="2">
         <v>0.13739999999999999</v>
+      </c>
+      <c r="I541" s="2">
+        <v>0.31272727272727269</v>
       </c>
       <c r="J541" s="2">
         <v>0.87000000000000011</v>
@@ -16616,8 +17543,14 @@
       <c r="F542" s="2">
         <v>-1.6439999999999995</v>
       </c>
+      <c r="G542" s="2">
+        <v>0.1164</v>
+      </c>
       <c r="H542" s="2">
         <v>0.12140000000000001</v>
+      </c>
+      <c r="I542" s="2">
+        <v>0.21478260869565219</v>
       </c>
       <c r="J542" s="2">
         <v>0.83000000000000007</v>
@@ -16642,8 +17575,14 @@
       <c r="F543" s="2">
         <v>-8.3789999999999996</v>
       </c>
+      <c r="G543" s="2">
+        <v>0.1208</v>
+      </c>
       <c r="H543" s="2">
         <v>0.21299999999999999</v>
+      </c>
+      <c r="I543" s="2">
+        <v>-1.0500000000000001E-2</v>
       </c>
       <c r="J543" s="2">
         <v>0.83000000000000007</v>
@@ -16668,8 +17607,14 @@
       <c r="F544" s="2">
         <v>-17.252000000000002</v>
       </c>
+      <c r="G544" s="2">
+        <v>0.1268</v>
+      </c>
       <c r="H544" s="2">
         <v>0.14630000000000001</v>
+      </c>
+      <c r="I544" s="2">
+        <v>0.58363636363636362</v>
       </c>
       <c r="J544" s="2">
         <v>1.27</v>
@@ -16694,8 +17639,14 @@
       <c r="F545" s="2">
         <v>17.263999999999999</v>
       </c>
+      <c r="G545" s="2">
+        <v>3.0000000000000003E-4</v>
+      </c>
       <c r="H545" s="2">
         <v>0.1171</v>
+      </c>
+      <c r="I545" s="2">
+        <v>0.49590909090909091</v>
       </c>
       <c r="J545" s="2">
         <v>1.6999999999999997</v>
@@ -16720,8 +17671,14 @@
       <c r="F546" s="2">
         <v>4.8850000000000007</v>
       </c>
+      <c r="G546" s="2">
+        <v>5.8999999999999999E-3</v>
+      </c>
       <c r="H546" s="2">
         <v>0.22109999999999999</v>
+      </c>
+      <c r="I546" s="2">
+        <v>0.52047619047619043</v>
       </c>
       <c r="J546" s="2">
         <v>1.4500000000000002</v>
@@ -16746,8 +17703,14 @@
       <c r="F547" s="2">
         <v>3.1160000000000001</v>
       </c>
+      <c r="G547" s="2">
+        <v>1.11E-2</v>
+      </c>
       <c r="H547" s="2">
         <v>0.11820000000000001</v>
+      </c>
+      <c r="I547" s="2">
+        <v>0.56909090909090909</v>
       </c>
       <c r="J547" s="2">
         <v>1.2000000000000002</v>
@@ -16772,8 +17735,14 @@
       <c r="F548" s="2">
         <v>2.504</v>
       </c>
+      <c r="G548" s="2">
+        <v>9.6000000000000009E-3</v>
+      </c>
       <c r="H548" s="2">
         <v>0.11499999999999999</v>
+      </c>
+      <c r="I548" s="2">
+        <v>0.47521739130434781</v>
       </c>
       <c r="J548" s="2">
         <v>1.17</v>
@@ -16798,8 +17767,14 @@
       <c r="F549" s="2">
         <v>5.9769999999999994</v>
       </c>
+      <c r="G549" s="2">
+        <v>7.899999999999999E-3</v>
+      </c>
       <c r="H549" s="2">
         <v>0.1754</v>
+      </c>
+      <c r="I549" s="2">
+        <v>0.54571428571428571</v>
       </c>
       <c r="J549" s="2">
         <v>1.02</v>
@@ -16824,8 +17799,14 @@
       <c r="F550" s="2">
         <v>-4.0190000000000001</v>
       </c>
+      <c r="G550" s="2">
+        <v>7.6000000000000009E-3</v>
+      </c>
       <c r="H550" s="2">
         <v>9.7599999999999992E-2</v>
+      </c>
+      <c r="I550" s="2">
+        <v>0.54500000000000004</v>
       </c>
       <c r="J550" s="2">
         <v>1.0499999999999998</v>
@@ -16850,8 +17831,14 @@
       <c r="F551" s="2">
         <v>-1.181</v>
       </c>
+      <c r="G551" s="2">
+        <v>7.3000000000000001E-3</v>
+      </c>
       <c r="H551" s="2">
         <v>0.10150000000000001</v>
+      </c>
+      <c r="I551" s="2">
+        <v>0.6554545454545454</v>
       </c>
       <c r="J551" s="2">
         <v>1.0899999999999999</v>
@@ -16876,8 +17863,14 @@
       <c r="F552" s="2">
         <v>17.505999999999997</v>
       </c>
+      <c r="G552" s="2">
+        <v>6.6000000000000008E-3</v>
+      </c>
       <c r="H552" s="2">
         <v>0.1767</v>
+      </c>
+      <c r="I552" s="2">
+        <v>0.70476190476190481</v>
       </c>
       <c r="J552" s="2">
         <v>1</v>
@@ -16902,8 +17895,14 @@
       <c r="F553" s="2">
         <v>5.431</v>
       </c>
+      <c r="G553" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
       <c r="H553" s="2">
         <v>0.1203</v>
+      </c>
+      <c r="I553" s="2">
+        <v>0.80956521739130438</v>
       </c>
       <c r="J553" s="2">
         <v>0.90000000000000036</v>
@@ -16928,8 +17927,14 @@
       <c r="F554" s="2">
         <v>-2.000000000000046E-3</v>
       </c>
+      <c r="G554" s="2">
+        <v>4.5999999999999999E-3</v>
+      </c>
       <c r="H554" s="2">
         <v>9.6799999999999997E-2</v>
+      </c>
+      <c r="I554" s="2">
+        <v>0.90238095238095239</v>
       </c>
       <c r="J554" s="2">
         <v>0.79</v>
@@ -16954,8 +17959,14 @@
       <c r="F555" s="2">
         <v>5.4369999999999994</v>
       </c>
+      <c r="G555" s="2">
+        <v>4.5000000000000005E-3</v>
+      </c>
       <c r="H555" s="2">
         <v>0.14400000000000002</v>
+      </c>
+      <c r="I555" s="2">
+        <v>1.1545000000000001</v>
       </c>
       <c r="J555" s="2">
         <v>0.71999999999999975</v>
@@ -16980,8 +17991,14 @@
       <c r="F556" s="2">
         <v>4.2920000000000016</v>
       </c>
+      <c r="G556" s="2">
+        <v>2.6999999999999997E-3</v>
+      </c>
       <c r="H556" s="2">
         <v>0.1109</v>
+      </c>
+      <c r="I556" s="2">
+        <v>1.579565217391304</v>
       </c>
       <c r="J556" s="2">
         <v>0.70000000000000018</v>
@@ -17006,8 +18023,14 @@
       <c r="F557" s="2">
         <v>4.721000000000001</v>
       </c>
+      <c r="G557" s="2">
+        <v>1.4E-3</v>
+      </c>
       <c r="H557" s="2">
         <v>8.1500000000000003E-2</v>
+      </c>
+      <c r="I557" s="2">
+        <v>1.614090909090909</v>
       </c>
       <c r="J557" s="2">
         <v>0.70000000000000018</v>
@@ -17032,8 +18055,14 @@
       <c r="F558" s="2">
         <v>0.43399999999999989</v>
       </c>
+      <c r="G558" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="H558" s="2">
         <v>0.14180000000000001</v>
+      </c>
+      <c r="I558" s="2">
+        <v>1.5266666666666671</v>
       </c>
       <c r="J558" s="2">
         <v>0.66000000000000014</v>
@@ -17058,8 +18087,14 @@
       <c r="F559" s="2">
         <v>2.5060000000000002</v>
       </c>
+      <c r="G559" s="2">
+        <v>3.9999999999999996E-4</v>
+      </c>
       <c r="H559" s="2">
         <v>9.1899999999999996E-2</v>
+      </c>
+      <c r="I559" s="2">
+        <v>1.4831818181818179</v>
       </c>
       <c r="J559" s="2">
         <v>0.64999999999999991</v>
@@ -17084,8 +18119,14 @@
       <c r="F560" s="2">
         <v>0.69800000000000006</v>
       </c>
+      <c r="G560" s="2">
+        <v>3.1000000000000003E-3</v>
+      </c>
       <c r="H560" s="2">
         <v>9.0200000000000002E-2</v>
+      </c>
+      <c r="I560" s="2">
+        <v>1.208636363636364</v>
       </c>
       <c r="J560" s="2">
         <v>0.67000000000000037</v>
@@ -17110,8 +18151,14 @@
       <c r="F561" s="2">
         <v>2.9459999999999997</v>
       </c>
+      <c r="G561" s="2">
+        <v>4.8999999999999998E-3</v>
+      </c>
       <c r="H561" s="2">
         <v>0.14050000000000001</v>
+      </c>
+      <c r="I561" s="2">
+        <v>1.228636363636364</v>
       </c>
       <c r="J561" s="2">
         <v>0.69000000000000039</v>
@@ -17136,8 +18183,14 @@
       <c r="F562" s="2">
         <v>-4.0840000000000005</v>
       </c>
+      <c r="G562" s="2">
+        <v>3.3000000000000004E-3</v>
+      </c>
       <c r="H562" s="2">
         <v>8.7400000000000005E-2</v>
+      </c>
+      <c r="I562" s="2">
+        <v>1.272272727272727</v>
       </c>
       <c r="J562" s="2">
         <v>0.70000000000000018</v>
@@ -17162,8 +18215,14 @@
       <c r="F563" s="2">
         <v>6.4959999999999996</v>
       </c>
+      <c r="G563" s="2">
+        <v>3.6999999999999997E-3</v>
+      </c>
       <c r="H563" s="2">
         <v>8.9899999999999994E-2</v>
+      </c>
+      <c r="I563" s="2">
+        <v>1.457619047619048</v>
       </c>
       <c r="J563" s="2">
         <v>0.66999999999999993</v>
@@ -17188,8 +18247,14 @@
       <c r="F564" s="2">
         <v>-2.3490000000000002</v>
       </c>
+      <c r="G564" s="2">
+        <v>4.4000000000000003E-3</v>
+      </c>
       <c r="H564" s="2">
         <v>0.14729999999999999</v>
+      </c>
+      <c r="I564" s="2">
+        <v>1.3709090909090911</v>
       </c>
       <c r="J564" s="2">
         <v>0.6599999999999997</v>
@@ -17214,8 +18279,14 @@
       <c r="F565" s="2">
         <v>3.0539999999999998</v>
       </c>
+      <c r="G565" s="2">
+        <v>6.7000000000000002E-3</v>
+      </c>
       <c r="H565" s="2">
         <v>9.8599999999999993E-2</v>
+      </c>
+      <c r="I565" s="2">
+        <v>1.3439130434782609</v>
       </c>
       <c r="J565" s="2">
         <v>0.64999999999999991</v>
@@ -17240,8 +18311,14 @@
       <c r="F566" s="2">
         <v>-5.8400000000000007</v>
       </c>
+      <c r="G566" s="2">
+        <v>4.4000000000000003E-3</v>
+      </c>
       <c r="H566" s="2">
         <v>7.8299999999999995E-2</v>
+      </c>
+      <c r="I566" s="2">
+        <v>1.5376190476190481</v>
       </c>
       <c r="J566" s="2">
         <v>0.64999999999999991</v>
@@ -17266,8 +18343,14 @@
       <c r="F567" s="2">
         <v>-2.3809999999999998</v>
       </c>
+      <c r="G567" s="2">
+        <v>2.8E-3</v>
+      </c>
       <c r="H567" s="2">
         <v>0.14200000000000002</v>
+      </c>
+      <c r="I567" s="2">
+        <v>1.528</v>
       </c>
       <c r="J567" s="2">
         <v>0.7200000000000002</v>
@@ -17292,8 +18375,14 @@
       <c r="F568" s="2">
         <v>2.3820000000000001</v>
       </c>
+      <c r="G568" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
       <c r="H568" s="2">
         <v>0.1116</v>
+      </c>
+      <c r="I568" s="2">
+        <v>1.6843478260869571</v>
       </c>
       <c r="J568" s="2">
         <v>0.85999999999999988</v>
@@ -17318,8 +18407,14 @@
       <c r="F569" s="2">
         <v>-9.8329999999999984</v>
       </c>
+      <c r="G569" s="2">
+        <v>3.6999999999999997E-3</v>
+      </c>
       <c r="H569" s="2">
         <v>7.8100000000000003E-2</v>
+      </c>
+      <c r="I569" s="2">
+        <v>1.89</v>
       </c>
       <c r="J569" s="2">
         <v>0.90000000000000036</v>
@@ -17344,8 +18439,14 @@
       <c r="F570" s="2">
         <v>-0.58200000000000007</v>
       </c>
+      <c r="G570" s="2">
+        <v>3.0699999999999998E-2</v>
+      </c>
       <c r="H570" s="2">
         <v>0.17570000000000002</v>
+      </c>
+      <c r="I570" s="2">
+        <v>1.8277272727272731</v>
       </c>
       <c r="J570" s="2">
         <v>0.99000000000000021</v>
@@ -17370,8 +18471,14 @@
       <c r="F571" s="2">
         <v>-8.9789999999999974</v>
       </c>
+      <c r="G571" s="2">
+        <v>5.67E-2</v>
+      </c>
       <c r="H571" s="2">
         <v>0.11379999999999998</v>
+      </c>
+      <c r="I571" s="2">
+        <v>1.5736363636363631</v>
       </c>
       <c r="J571" s="2">
         <v>1.0299999999999994</v>
@@ -17396,8 +18503,14 @@
       <c r="F572" s="2">
         <v>10.015000000000001</v>
       </c>
+      <c r="G572" s="2">
+        <v>8.1199999999999994E-2</v>
+      </c>
       <c r="H572" s="2">
         <v>0.1008</v>
+      </c>
+      <c r="I572" s="2">
+        <v>0.63190476190476186</v>
       </c>
       <c r="J572" s="2">
         <v>1.1500000000000004</v>
@@ -17422,8 +18535,14 @@
       <c r="F573" s="2">
         <v>-3.4769999999999994</v>
       </c>
+      <c r="G573" s="2">
+        <v>0.19009999999999999</v>
+      </c>
       <c r="H573" s="2">
         <v>0.1794</v>
+      </c>
+      <c r="I573" s="2">
+        <v>0.26695652173913043</v>
       </c>
       <c r="J573" s="2">
         <v>1.08</v>
@@ -17448,8 +18567,14 @@
       <c r="F574" s="2">
         <v>-9.3719999999999981</v>
       </c>
+      <c r="G574" s="2">
+        <v>0.19289999999999999</v>
+      </c>
       <c r="H574" s="2">
         <v>0.11169999999999999</v>
+      </c>
+      <c r="I574" s="2">
+        <v>0.37454545454545463</v>
       </c>
       <c r="J574" s="2">
         <v>1.1000000000000005</v>
@@ -17474,8 +18599,14 @@
       <c r="F575" s="2">
         <v>8.597999999999999</v>
       </c>
+      <c r="G575" s="2">
+        <v>0.23270000000000002</v>
+      </c>
       <c r="H575" s="2">
         <v>0.1109</v>
+      </c>
+      <c r="I575" s="2">
+        <v>0.25380952380952371</v>
       </c>
       <c r="J575" s="2">
         <v>1.1600000000000001</v>
@@ -17500,8 +18631,14 @@
       <c r="F576" s="2">
         <v>5.104000000000001</v>
       </c>
+      <c r="G576" s="2">
+        <v>0.28560000000000002</v>
+      </c>
       <c r="H576" s="2">
         <v>0.20400000000000001</v>
+      </c>
+      <c r="I576" s="2">
+        <v>-0.23681818181818179</v>
       </c>
       <c r="J576" s="2">
         <v>1.17</v>
@@ -17526,8 +18663,14 @@
       <c r="F577" s="2">
         <v>-6.1229999999999993</v>
       </c>
+      <c r="G577" s="2">
+        <v>0.33789999999999998</v>
+      </c>
       <c r="H577" s="2">
         <v>0.1132</v>
+      </c>
+      <c r="I577" s="2">
+        <v>-0.6072727272727273</v>
       </c>
       <c r="J577" s="2">
         <v>1.1600000000000001</v>
@@ -17552,8 +18695,14 @@
       <c r="F578" s="2">
         <v>8.3260000000000005</v>
       </c>
+      <c r="G578" s="2">
+        <v>0.35060000000000002</v>
+      </c>
       <c r="H578" s="2">
         <v>0.1</v>
+      </c>
+      <c r="I578" s="2">
+        <v>-0.91454545454545455</v>
       </c>
       <c r="J578" s="2">
         <v>1.0999999999999996</v>
@@ -17578,8 +18727,14 @@
       <c r="F579" s="2">
         <v>-1.847</v>
       </c>
+      <c r="G579" s="2">
+        <v>0.34499999999999997</v>
+      </c>
       <c r="H579" s="2">
         <v>0.1749</v>
+      </c>
+      <c r="I579" s="2">
+        <v>-0.86250000000000004</v>
       </c>
       <c r="J579" s="2">
         <v>1.0300000000000002</v>
@@ -17604,8 +18759,14 @@
       <c r="F580" s="2">
         <v>2.0810000000000004</v>
       </c>
+      <c r="G580" s="2">
+        <v>0.36380000000000001</v>
+      </c>
       <c r="H580" s="2">
         <v>0.1358</v>
+      </c>
+      <c r="I580" s="2">
+        <v>-1.028695652173913</v>
       </c>
       <c r="J580" s="2">
         <v>1.1100000000000003</v>
@@ -17630,8 +18791,14 @@
       <c r="F581" s="2">
         <v>0.61999999999999988</v>
       </c>
+      <c r="G581" s="2">
+        <v>0.36399999999999999</v>
+      </c>
       <c r="H581" s="2">
         <v>9.0899999999999995E-2</v>
+      </c>
+      <c r="I581" s="2">
+        <v>-1.4644999999999999</v>
       </c>
       <c r="J581" s="2">
         <v>1.0600000000000005</v>
@@ -17656,8 +18823,14 @@
       <c r="F582" s="2">
         <v>1.7759999999999998</v>
       </c>
+      <c r="G582" s="2">
+        <v>0.36619999999999997</v>
+      </c>
       <c r="H582" s="2">
         <v>0.1888</v>
+      </c>
+      <c r="I582" s="2">
+        <v>-1.493913043478261</v>
       </c>
       <c r="J582" s="2">
         <v>1.0999999999999996</v>
@@ -17682,8 +18855,14 @@
       <c r="F583" s="2">
         <v>7.5449999999999999</v>
       </c>
+      <c r="G583" s="2">
+        <v>0.4078</v>
+      </c>
       <c r="H583" s="2">
         <v>0.10560000000000001</v>
+      </c>
+      <c r="I583" s="2">
+        <v>-1.3459090909090909</v>
       </c>
       <c r="J583" s="2">
         <v>1.0999999999999996</v>
@@ -17708,8 +18887,14 @@
       <c r="F584" s="2">
         <v>4.8230000000000004</v>
       </c>
+      <c r="G584" s="2">
+        <v>0.43909999999999999</v>
+      </c>
       <c r="H584" s="2">
         <v>9.169999999999999E-2</v>
+      </c>
+      <c r="I584" s="2">
+        <v>-1.29</v>
       </c>
       <c r="J584" s="2">
         <v>1.08</v>
@@ -17734,8 +18919,14 @@
       <c r="F585" s="2">
         <v>-2.8230000000000004</v>
       </c>
+      <c r="G585" s="2">
+        <v>0.45370000000000005</v>
+      </c>
       <c r="H585" s="2">
         <v>0.17880000000000001</v>
+      </c>
+      <c r="I585" s="2">
+        <v>-1.1286956521739131</v>
       </c>
       <c r="J585" s="2">
         <v>1.0699999999999994</v>
@@ -17760,8 +18951,14 @@
       <c r="F586" s="2">
         <v>-5.1039999999999992</v>
       </c>
+      <c r="G586" s="2">
+        <v>0.42669999999999997</v>
+      </c>
       <c r="H586" s="2">
         <v>8.4500000000000006E-2</v>
+      </c>
+      <c r="I586" s="2">
+        <v>-0.8957142857142858</v>
       </c>
       <c r="J586" s="2">
         <v>1.0300000000000002</v>
@@ -17786,8 +18983,14 @@
       <c r="F587" s="2">
         <v>-3.5859999999999999</v>
       </c>
+      <c r="G587" s="2">
+        <v>0.47149999999999997</v>
+      </c>
       <c r="H587" s="2">
         <v>9.3600000000000003E-2</v>
+      </c>
+      <c r="I587" s="2">
+        <v>-0.51272727272727259</v>
       </c>
       <c r="J587" s="2">
         <v>1.0199999999999996</v>
@@ -17812,8 +19015,14 @@
       <c r="F588" s="2">
         <v>8.9030000000000005</v>
       </c>
+      <c r="G588" s="2">
+        <v>0.44240000000000002</v>
+      </c>
       <c r="H588" s="2">
         <v>0.21649999999999997</v>
+      </c>
+      <c r="I588" s="2">
+        <v>-0.7322727272727273</v>
       </c>
       <c r="J588" s="2">
         <v>1.0099999999999998</v>
@@ -17838,8 +19047,14 @@
       <c r="F589" s="2">
         <v>7.3259999999999987</v>
       </c>
+      <c r="G589" s="2">
+        <v>0.42659999999999998</v>
+      </c>
       <c r="H589" s="2">
         <v>0.11150000000000002</v>
+      </c>
+      <c r="I589" s="2">
+        <v>-1.1633333333333331</v>
       </c>
       <c r="J589" s="2">
         <v>0.89999999999999947</v>

</xml_diff>